<commit_message>
ook 1.0 van het Excel bijgewerkt, TPOD2070 weet ik nog niet of deze voor 1.0 geldt.
</commit_message>
<xml_diff>
--- a/1.0-Validatie-_en_conformiteitsregels_TPOD/documentatie/Validatie-en-Conformiteitsregels Totaal v0.10 - incl onderscheidOntwerpDefinitief.xlsx
+++ b/1.0-Validatie-_en_conformiteitsregels_TPOD/documentatie/Validatie-en-Conformiteitsregels Totaal v0.10 - incl onderscheidOntwerpDefinitief.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Default.DESKTOP-NDDI22K\Documents\Geonovum\github\xml_schematron\1.0-Validatie-_en_conformiteitsregels_TPOD\documentatie\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RicharddeGraaf\Desktop\Geonovum\4 - Voorbeeldbestanden\GITHub\xml_schematron\1.0-Validatie-_en_conformiteitsregels_TPOD\documentatie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDFE03F7-A7F8-4E2E-892D-E1D654E93427}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41D0A0D2-9F7D-4403-B1BD-C607AFC9FB09}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="348" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{CAF58E0D-33FE-46EB-ADA3-90D1B902B379}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{CAF58E0D-33FE-46EB-ADA3-90D1B902B379}"/>
   </bookViews>
   <sheets>
     <sheet name="TotaalOverzicht" sheetId="6" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13876" uniqueCount="675">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13922" uniqueCount="680">
   <si>
     <t>ID</t>
   </si>
@@ -2113,12 +2113,56 @@
   <si>
     <t>De nummering van Artikelen begint met het nummer van het Hoofdstuk waarin het Artikel voorkomt, gevolgd door een punt, daarna oplopende nummering van de Artikelen in Arabische cijfers inclusief indien nodig een letter</t>
   </si>
+  <si>
+    <t>Ieder OwObject heeft minstens een OwObject dat ernaar verwijst.</t>
+  </si>
+  <si>
+    <t>TPOD2060</t>
+  </si>
+  <si>
+    <t>Als een verwijzing naar een Lid is gemaakt mag er geen verwijzing meer gemaakt worden naar het artikel dat boven dit Lid hangt. (RegeltekstID alleen op Lid-niveau of alleen op Artikel-niveau.)</t>
+  </si>
+  <si>
+    <t>TPOD2070</t>
+  </si>
+  <si>
+    <r>
+      <t>Als de activiteit een bepaalde regeltekstID heeft dan moet deze overeenkomen met de ID die je via de logische relaties vindt (regeltekst naar</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> juridische regel (regel voor iedereen) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Wingdings"/>
+        <charset val="2"/>
+      </rPr>
+      <t>naar</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> activiteitaanduiding).</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -2186,8 +2230,20 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Wingdings"/>
+      <charset val="2"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2227,6 +2283,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2412,9 +2474,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -2435,12 +2494,25 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
     <cellStyle name="Standaard 2" xfId="1" xr:uid="{DD73F50D-CE68-4CBD-BD67-3376699AD112}"/>
   </cellStyles>
-  <dxfs count="123">
+  <dxfs count="124">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FFFF0000"/>
@@ -25156,247 +25228,247 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C169:F197 G167:H197 D198:D251 E198:E250 C198:C238 F198:H251 G252:H271 A28:A29 A1:E27 A152:H152 A30:F48 A59:H126 G1:V1 G2:H48 J2:J48 J59:J126 L59:L126 L2:L48 N2:N48 N59:N126 J152 J167:J271 L167:L271 L152 N152 N167:N271 P167:P271 P152 P59:P126 P2:P48 R2:R48 R59:R126 R152 T152 T59:T126 T2:T48 V2:V48 V59:V126 V152">
-    <cfRule type="containsText" dxfId="122" priority="63" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="123" priority="63" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28:E29 F1:F29">
-    <cfRule type="containsText" dxfId="121" priority="62" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="122" priority="62" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B28">
-    <cfRule type="containsText" dxfId="120" priority="61" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="121" priority="61" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B28)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B29">
-    <cfRule type="containsText" dxfId="119" priority="60" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="120" priority="60" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B29)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C252:C271">
-    <cfRule type="containsText" dxfId="118" priority="45" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="119" priority="45" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C252)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C167:F168 D252:F271">
-    <cfRule type="containsText" dxfId="117" priority="59" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="118" priority="59" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C167)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C251 E251">
-    <cfRule type="containsText" dxfId="116" priority="46" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="117" priority="46" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C251)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C239">
-    <cfRule type="containsText" dxfId="115" priority="58" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="116" priority="58" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C239)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C240">
-    <cfRule type="containsText" dxfId="114" priority="57" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="115" priority="57" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C240)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C241">
-    <cfRule type="containsText" dxfId="113" priority="56" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="114" priority="56" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C241)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C242">
-    <cfRule type="containsText" dxfId="112" priority="55" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="113" priority="55" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C242)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C243">
-    <cfRule type="containsText" dxfId="111" priority="54" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="112" priority="54" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C243)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C244">
-    <cfRule type="containsText" dxfId="110" priority="53" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="111" priority="53" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C244)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C245">
-    <cfRule type="containsText" dxfId="109" priority="52" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="110" priority="52" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C245)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C246">
-    <cfRule type="containsText" dxfId="108" priority="51" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="109" priority="51" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C246)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C247">
-    <cfRule type="containsText" dxfId="107" priority="50" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="108" priority="50" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C247)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C248">
-    <cfRule type="containsText" dxfId="106" priority="49" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="107" priority="49" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C248)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C249">
-    <cfRule type="containsText" dxfId="105" priority="48" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="106" priority="48" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C249)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C250">
-    <cfRule type="containsText" dxfId="104" priority="47" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="105" priority="47" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C250)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A49:E53 G49:H53 J49:J53 L49:L53 N49:N53 P49:P53 R49:R53 T49:T53 V49:V53">
-    <cfRule type="containsText" dxfId="103" priority="39" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="104" priority="39" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",A49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F49:F53">
-    <cfRule type="containsText" dxfId="102" priority="38" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="103" priority="38" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",F49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A54:E58 G54:H58 J54:J58 L54:L58 N54:N58 P54:P58 R54:R58 T54:T58 V54:V58">
-    <cfRule type="containsText" dxfId="101" priority="37" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="102" priority="37" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",A54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F54:F58">
-    <cfRule type="containsText" dxfId="100" priority="36" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="101" priority="36" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",F54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2:Q48 Q59:Q126 Q152">
-    <cfRule type="containsText" dxfId="99" priority="14" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="100" priority="14" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",Q2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q49:Q53">
-    <cfRule type="containsText" dxfId="98" priority="13" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="99" priority="13" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",Q49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q54:Q58">
-    <cfRule type="containsText" dxfId="97" priority="12" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="98" priority="12" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",Q54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S54:S58">
-    <cfRule type="containsText" dxfId="96" priority="9" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="97" priority="9" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",S54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U2:U48 U59:U126 U152">
-    <cfRule type="containsText" dxfId="95" priority="8" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="96" priority="8" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",U2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U49:U53">
-    <cfRule type="containsText" dxfId="94" priority="7" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="95" priority="7" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",U49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U54:U58">
-    <cfRule type="containsText" dxfId="93" priority="6" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="94" priority="6" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",U54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q167:Q271">
-    <cfRule type="containsText" dxfId="92" priority="1" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="93" priority="1" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",Q167)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I48 I59:I126 I152 I167:I271">
-    <cfRule type="containsText" dxfId="91" priority="26" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="92" priority="26" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",I2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I49:I53">
-    <cfRule type="containsText" dxfId="90" priority="25" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="91" priority="25" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",I49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I54:I58">
-    <cfRule type="containsText" dxfId="89" priority="24" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="90" priority="24" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",I54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K59:K126 K2:K48 K167:K271 K152">
-    <cfRule type="containsText" dxfId="88" priority="23" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="89" priority="23" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",K2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K49:K53">
-    <cfRule type="containsText" dxfId="87" priority="22" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="88" priority="22" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",K49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K54:K58">
-    <cfRule type="containsText" dxfId="86" priority="21" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="87" priority="21" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",K54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M48 M59:M126 M152 M167:M271">
-    <cfRule type="containsText" dxfId="85" priority="20" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="86" priority="20" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M49:M53">
-    <cfRule type="containsText" dxfId="84" priority="19" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="85" priority="19" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M54:M58">
-    <cfRule type="containsText" dxfId="83" priority="18" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="84" priority="18" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O167:O271 O152 O59:O126 O2:O48">
-    <cfRule type="containsText" dxfId="82" priority="17" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="83" priority="17" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",O2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O49:O53">
-    <cfRule type="containsText" dxfId="81" priority="16" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="82" priority="16" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",O49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O54:O58">
-    <cfRule type="containsText" dxfId="80" priority="15" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="81" priority="15" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",O54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S152 S59:S126 S2:S48">
-    <cfRule type="containsText" dxfId="79" priority="11" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="80" priority="11" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",S2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S49:S53">
-    <cfRule type="containsText" dxfId="78" priority="10" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="79" priority="10" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",S49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V167:V271 T167:T271">
-    <cfRule type="containsText" dxfId="77" priority="5" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="78" priority="5" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",T167)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U167:U271">
-    <cfRule type="containsText" dxfId="76" priority="4" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="77" priority="4" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",U167)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S167:S271">
-    <cfRule type="containsText" dxfId="75" priority="3" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="76" priority="3" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",S167)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R167:R271">
-    <cfRule type="containsText" dxfId="74" priority="2" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="75" priority="2" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",R167)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -29397,147 +29469,147 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="O2:O48">
-    <cfRule type="containsText" dxfId="73" priority="12" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="74" priority="12" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",O2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O49:O53">
-    <cfRule type="containsText" dxfId="72" priority="11" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="73" priority="11" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",O49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S2:S48">
-    <cfRule type="containsText" dxfId="71" priority="6" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="72" priority="6" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",S2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S49:S53">
-    <cfRule type="containsText" dxfId="70" priority="5" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="71" priority="5" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",S49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q49:Q53">
-    <cfRule type="containsText" dxfId="69" priority="8" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="70" priority="8" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",Q49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q54:Q58">
-    <cfRule type="containsText" dxfId="68" priority="7" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="69" priority="7" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",Q54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U54:U58">
-    <cfRule type="containsText" dxfId="67" priority="1" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="68" priority="1" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",U54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S54:S58">
-    <cfRule type="containsText" dxfId="66" priority="4" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="67" priority="4" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",S54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U2:U48">
-    <cfRule type="containsText" dxfId="65" priority="3" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="66" priority="3" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",U2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U49:U53">
-    <cfRule type="containsText" dxfId="64" priority="2" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="65" priority="2" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",U49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A28:A29 A1:E27 A30:F48 G1:V1 G2:H48 J2:J48 L2:L48 N2:N48 P2:P48 R2:R48 T2:T48 V2:V48">
-    <cfRule type="containsText" dxfId="63" priority="29" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="64" priority="29" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28:E29 F1:F29">
-    <cfRule type="containsText" dxfId="62" priority="28" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="63" priority="28" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B28">
-    <cfRule type="containsText" dxfId="61" priority="27" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="62" priority="27" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B28)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B29">
-    <cfRule type="containsText" dxfId="60" priority="26" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="61" priority="26" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B29)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A49:E53 G49:H53 J49:J53 L49:L53 N49:N53 P49:P53 R49:R53 T49:T53 V49:V53">
-    <cfRule type="containsText" dxfId="59" priority="25" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="60" priority="25" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",A49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F49:F53">
-    <cfRule type="containsText" dxfId="58" priority="24" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="59" priority="24" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",F49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A54:E58 G54:H58 J54:J58 L54:L58 N54:N58 P54:P58 R54:R58 T54:T58 V54:V58">
-    <cfRule type="containsText" dxfId="57" priority="23" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="58" priority="23" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",A54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F54:F58">
-    <cfRule type="containsText" dxfId="56" priority="22" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="57" priority="22" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",F54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2:Q48">
-    <cfRule type="containsText" dxfId="55" priority="9" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="56" priority="9" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",Q2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I48">
-    <cfRule type="containsText" dxfId="54" priority="21" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="55" priority="21" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",I2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I49:I53">
-    <cfRule type="containsText" dxfId="53" priority="20" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="54" priority="20" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",I49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I54:I58">
-    <cfRule type="containsText" dxfId="52" priority="19" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="53" priority="19" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",I54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K48">
-    <cfRule type="containsText" dxfId="51" priority="18" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="52" priority="18" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",K2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K49:K53">
-    <cfRule type="containsText" dxfId="50" priority="17" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="51" priority="17" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",K49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K54:K58">
-    <cfRule type="containsText" dxfId="49" priority="16" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="50" priority="16" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",K54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M48">
-    <cfRule type="containsText" dxfId="48" priority="15" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="49" priority="15" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M49:M53">
-    <cfRule type="containsText" dxfId="47" priority="14" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="48" priority="14" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M54:M58">
-    <cfRule type="containsText" dxfId="46" priority="13" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="47" priority="13" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O54:O58">
-    <cfRule type="containsText" dxfId="45" priority="10" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="46" priority="10" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",O54)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -29567,8 +29639,8 @@
   <dimension ref="A1:W217"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B56" sqref="B56"/>
+      <pane ySplit="1" topLeftCell="A107" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B118" sqref="B118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -29586,7 +29658,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="59" t="s">
         <v>672</v>
       </c>
       <c r="B1" s="22" t="s">
@@ -29791,7 +29863,7 @@
       </c>
     </row>
     <row r="4" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="57" t="s">
+      <c r="B4" s="56" t="s">
         <v>560</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -30533,7 +30605,7 @@
       </c>
     </row>
     <row r="15" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="57" t="s">
+      <c r="B15" s="56" t="s">
         <v>530</v>
       </c>
       <c r="C15" s="2" t="s">
@@ -30871,7 +30943,7 @@
       </c>
     </row>
     <row r="20" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="57" t="s">
+      <c r="B20" s="56" t="s">
         <v>534</v>
       </c>
       <c r="C20" s="2" t="s">
@@ -31277,7 +31349,7 @@
       </c>
     </row>
     <row r="26" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="57" t="s">
+      <c r="B26" s="56" t="s">
         <v>539</v>
       </c>
       <c r="C26" s="2" t="s">
@@ -31613,7 +31685,7 @@
       </c>
     </row>
     <row r="31" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="57" t="s">
+      <c r="B31" s="56" t="s">
         <v>542</v>
       </c>
       <c r="C31" s="2" t="s">
@@ -31949,7 +32021,7 @@
       </c>
     </row>
     <row r="36" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="57" t="s">
+      <c r="B36" s="56" t="s">
         <v>545</v>
       </c>
       <c r="C36" s="2" t="s">
@@ -32353,7 +32425,7 @@
       </c>
     </row>
     <row r="42" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="57" t="s">
+      <c r="B42" s="56" t="s">
         <v>549</v>
       </c>
       <c r="C42" s="2" t="s">
@@ -36111,7 +36183,7 @@
       </c>
     </row>
     <row r="98" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B98" s="56" t="s">
+      <c r="B98" s="55" t="s">
         <v>137</v>
       </c>
       <c r="C98" s="3" t="s">
@@ -36179,7 +36251,7 @@
       </c>
     </row>
     <row r="99" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B99" s="57" t="s">
+      <c r="B99" s="56" t="s">
         <v>137</v>
       </c>
       <c r="C99" s="2" t="s">
@@ -36862,11 +36934,11 @@
       </c>
     </row>
     <row r="109" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B109" s="52" t="s">
+      <c r="B109" s="60" t="s">
         <v>641</v>
       </c>
-      <c r="C109" s="53" t="s">
-        <v>642</v>
+      <c r="C109" s="52" t="s">
+        <v>675</v>
       </c>
       <c r="D109" s="3" t="s">
         <v>123</v>
@@ -36930,10 +37002,10 @@
       </c>
     </row>
     <row r="110" spans="1:23" ht="110.4" x14ac:dyDescent="0.3">
-      <c r="B110" s="58" t="s">
+      <c r="B110" s="57" t="s">
         <v>667</v>
       </c>
-      <c r="C110" s="54" t="s">
+      <c r="C110" s="53" t="s">
         <v>662</v>
       </c>
       <c r="D110" s="32" t="s">
@@ -36998,7 +37070,7 @@
       </c>
     </row>
     <row r="111" spans="1:23" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="B111" s="59" t="s">
+      <c r="B111" s="58" t="s">
         <v>661</v>
       </c>
       <c r="C111" s="36" t="s">
@@ -37066,7 +37138,7 @@
       </c>
     </row>
     <row r="112" spans="1:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B112" s="59" t="s">
+      <c r="B112" s="58" t="s">
         <v>668</v>
       </c>
       <c r="C112" s="36" t="s">
@@ -37133,8 +37205,8 @@
         <v>134</v>
       </c>
     </row>
-    <row r="113" spans="2:23" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="B113" s="59" t="s">
+    <row r="113" spans="1:23" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="B113" s="58" t="s">
         <v>669</v>
       </c>
       <c r="C113" s="36" t="s">
@@ -37201,8 +37273,8 @@
         <v>134</v>
       </c>
     </row>
-    <row r="114" spans="2:23" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="B114" s="59" t="s">
+    <row r="114" spans="1:23" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="B114" s="58" t="s">
         <v>670</v>
       </c>
       <c r="C114" s="36" t="s">
@@ -37269,11 +37341,11 @@
         <v>134</v>
       </c>
     </row>
-    <row r="115" spans="2:23" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:23" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B115" s="31" t="s">
         <v>671</v>
       </c>
-      <c r="C115" s="55" t="s">
+      <c r="C115" s="54" t="s">
         <v>660</v>
       </c>
       <c r="D115" s="32" t="s">
@@ -37337,43 +37409,179 @@
         <v>134</v>
       </c>
     </row>
-    <row r="116" spans="2:23" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="B116" s="45"/>
-    </row>
-    <row r="117" spans="2:23" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="B117" s="45"/>
-    </row>
-    <row r="118" spans="2:23" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:23" s="26" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A116" s="1" t="s">
+        <v>676</v>
+      </c>
+      <c r="B116" s="54" t="s">
+        <v>676</v>
+      </c>
+      <c r="C116" s="54" t="s">
+        <v>677</v>
+      </c>
+      <c r="D116" s="32" t="s">
+        <v>123</v>
+      </c>
+      <c r="E116" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="F116" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="G116" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="H116" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="I116" s="3" t="s">
+        <v>643</v>
+      </c>
+      <c r="J116" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="K116" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="L116" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="M116" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="N116" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="O116" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="P116" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q116" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="R116" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="S116" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="T116" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="U116" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="V116" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="W116" s="19" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="117" spans="1:23" s="26" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A117" s="1" t="s">
+        <v>678</v>
+      </c>
+      <c r="B117" s="54" t="s">
+        <v>678</v>
+      </c>
+      <c r="C117" s="54" t="s">
+        <v>679</v>
+      </c>
+      <c r="D117" s="32" t="s">
+        <v>123</v>
+      </c>
+      <c r="E117" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="F117" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="G117" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="H117" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="I117" s="3" t="s">
+        <v>643</v>
+      </c>
+      <c r="J117" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="K117" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="L117" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="M117" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="N117" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="O117" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="P117" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q117" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="R117" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="S117" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="T117" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="U117" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="V117" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="W117" s="19" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="118" spans="1:23" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B118" s="45"/>
     </row>
-    <row r="119" spans="2:23" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:23" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B119" s="45"/>
     </row>
-    <row r="120" spans="2:23" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:23" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B120" s="45"/>
     </row>
-    <row r="121" spans="2:23" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:23" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B121" s="45"/>
     </row>
-    <row r="122" spans="2:23" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:23" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B122" s="45"/>
     </row>
-    <row r="123" spans="2:23" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:23" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B123" s="45"/>
     </row>
-    <row r="124" spans="2:23" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:23" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B124" s="45"/>
     </row>
-    <row r="125" spans="2:23" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:23" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B125" s="45"/>
     </row>
-    <row r="126" spans="2:23" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:23" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B126" s="45"/>
     </row>
-    <row r="127" spans="2:23" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:23" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B127" s="45"/>
     </row>
-    <row r="128" spans="2:23" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:23" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B128" s="45"/>
     </row>
     <row r="129" spans="2:2" ht="13.8" x14ac:dyDescent="0.25">
@@ -37645,63 +37853,68 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B96:I96 B2:I69">
-    <cfRule type="containsText" dxfId="44" priority="24" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="45" priority="25" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T95 T2:T69">
-    <cfRule type="containsText" dxfId="43" priority="2" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="44" priority="3" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",T2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V2:V69 V95">
-    <cfRule type="containsText" dxfId="42" priority="1" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="43" priority="2" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",V2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:F1 H1:W1">
-    <cfRule type="containsText" dxfId="41" priority="20" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="42" priority="21" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1">
-    <cfRule type="containsText" dxfId="40" priority="19" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="41" priority="20" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B202 B116:B176">
-    <cfRule type="containsText" dxfId="39" priority="18" operator="containsText" text="&lt;?&gt;">
-      <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B116)))</formula>
+  <conditionalFormatting sqref="B202 B118:B176">
+    <cfRule type="containsText" dxfId="40" priority="19" operator="containsText" text="&lt;?&gt;">
+      <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B118)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K69 M2:M69 O2:O69 K95 M95 O95 Q95 Q2:Q69 S2:S69 S95 U95 U2:U69 W2:W69 W95">
-    <cfRule type="containsText" dxfId="38" priority="8" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="39" priority="9" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",K2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R2:R69 R95">
-    <cfRule type="containsText" dxfId="37" priority="3" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="38" priority="4" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",R2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J69 J95">
-    <cfRule type="containsText" dxfId="36" priority="7" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="37" priority="8" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",J2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:L69 L95">
-    <cfRule type="containsText" dxfId="35" priority="6" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="36" priority="7" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",L2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2:N69 N95">
-    <cfRule type="containsText" dxfId="34" priority="5" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="35" priority="6" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",N2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P95 P2:P69">
-    <cfRule type="containsText" dxfId="33" priority="4" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="34" priority="5" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",P2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A116:A117">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="&lt;?&gt;">
+      <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",A116)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -44956,137 +45169,137 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:E1 G1:H1">
-    <cfRule type="containsText" dxfId="32" priority="27" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="33" priority="27" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1">
-    <cfRule type="containsText" dxfId="31" priority="26" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="32" priority="26" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",F1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:F32 D33:D86 E33:E85 C33:C73 G2:H32 F33:H86 G87:H106 V2:V106 T2:T106 R2:R106">
-    <cfRule type="containsText" dxfId="30" priority="25" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="31" priority="25" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C87:C106">
-    <cfRule type="containsText" dxfId="29" priority="10" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="30" priority="10" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C87)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:F3 D87:F106">
-    <cfRule type="containsText" dxfId="28" priority="24" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="29" priority="24" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C86 E86">
-    <cfRule type="containsText" dxfId="27" priority="11" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="28" priority="11" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C86)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C74">
-    <cfRule type="containsText" dxfId="26" priority="23" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="27" priority="23" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C74)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C75">
-    <cfRule type="containsText" dxfId="25" priority="22" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="26" priority="22" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C75)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C76">
-    <cfRule type="containsText" dxfId="24" priority="21" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="25" priority="21" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C76)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C77">
-    <cfRule type="containsText" dxfId="23" priority="20" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="24" priority="20" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C77)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C78">
-    <cfRule type="containsText" dxfId="22" priority="19" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="23" priority="19" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C78)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C79">
-    <cfRule type="containsText" dxfId="21" priority="18" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="22" priority="18" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C79)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C80">
-    <cfRule type="containsText" dxfId="20" priority="17" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="21" priority="17" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C80)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C81">
-    <cfRule type="containsText" dxfId="19" priority="16" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="20" priority="16" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C81)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C82">
-    <cfRule type="containsText" dxfId="18" priority="15" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="19" priority="15" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C82)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C83">
-    <cfRule type="containsText" dxfId="17" priority="14" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="18" priority="14" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C83)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C84">
-    <cfRule type="containsText" dxfId="16" priority="13" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="17" priority="13" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C84)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C85">
-    <cfRule type="containsText" dxfId="15" priority="12" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="16" priority="12" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C85)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:V1">
-    <cfRule type="containsText" dxfId="14" priority="9" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="15" priority="9" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",I1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U2:U106">
-    <cfRule type="containsText" dxfId="13" priority="8" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="14" priority="8" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",U2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S2:S106">
-    <cfRule type="containsText" dxfId="12" priority="7" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="13" priority="7" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",S2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2:Q106">
-    <cfRule type="containsText" dxfId="11" priority="6" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="12" priority="6" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",Q2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J106 L2:L106 N2:N106 P2:P106">
-    <cfRule type="containsText" dxfId="10" priority="5" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="11" priority="5" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",J2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I106">
-    <cfRule type="containsText" dxfId="9" priority="4" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="10" priority="4" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",I2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K106">
-    <cfRule type="containsText" dxfId="8" priority="3" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="9" priority="3" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",K2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M106">
-    <cfRule type="containsText" dxfId="7" priority="2" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="8" priority="2" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O2:O106">
-    <cfRule type="containsText" dxfId="6" priority="1" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="7" priority="1" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",O2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -45943,17 +46156,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:E1 G1:H1">
-    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="6" priority="4" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1">
-    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",F1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:V1">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",I1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -48092,17 +48305,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:E1 G1:H1">
-    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1">
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",F1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:V1">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",I1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
documentatie aangepast naar nieuwe constraints in 1.0
</commit_message>
<xml_diff>
--- a/1.0-Validatie-_en_conformiteitsregels_TPOD/documentatie/Validatie-en-Conformiteitsregels Totaal v0.10 - incl onderscheidOntwerpDefinitief.xlsx
+++ b/1.0-Validatie-_en_conformiteitsregels_TPOD/documentatie/Validatie-en-Conformiteitsregels Totaal v0.10 - incl onderscheidOntwerpDefinitief.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Default.DESKTOP-NDDI22K\Documents\Geonovum\github\xml_schematron\1.0-Validatie-_en_conformiteitsregels_TPOD\documentatie\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RicharddeGraaf\Desktop\Geonovum\4 - Voorbeeldbestanden\GITHub\xml_schematron\1.0-Validatie-_en_conformiteitsregels_TPOD\documentatie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{603C4FC2-E970-4440-8603-4B736ED70E77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FB09E9D-670F-4AAA-A66D-0BD194BC049A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="348" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{CAF58E0D-33FE-46EB-ADA3-90D1B902B379}"/>
+    <workbookView xWindow="732" yWindow="732" windowWidth="18552" windowHeight="11028" activeTab="2" xr2:uid="{CAF58E0D-33FE-46EB-ADA3-90D1B902B379}"/>
   </bookViews>
   <sheets>
     <sheet name="TotaalOverzicht" sheetId="6" r:id="rId1"/>
@@ -24,7 +24,6 @@
     <externalReference r:id="rId7"/>
   </externalReferences>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -42,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13920" uniqueCount="680">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14052" uniqueCount="693">
   <si>
     <t>ID</t>
   </si>
@@ -2117,6 +2116,45 @@
   </si>
   <si>
     <t>Ieder OwObject heeft minstens een OwObject dat ernaar verwijst.</t>
+  </si>
+  <si>
+    <t>TPOD2080</t>
+  </si>
+  <si>
+    <t>Binnen een instructieregel dient er gekozen te worden tussen InstructieregelInstrument of InstructieregelTaakuitoefening (één van de twee moet voorkomen, niet meer, niet minder).</t>
+  </si>
+  <si>
+    <t>1.0</t>
+  </si>
+  <si>
+    <t>TPOD2090</t>
+  </si>
+  <si>
+    <t>Alle normwaarden van een norm moeten hetzelfde type zijn (kwalitatief, kwantitatief, of waardeInRegeltekst).</t>
+  </si>
+  <si>
+    <t>TPOD2100</t>
+  </si>
+  <si>
+    <t>Eenheid mag alleen voorkomen bij een Norm die kwantitatieve normwaarden heeft</t>
+  </si>
+  <si>
+    <t>TPOD2110</t>
+  </si>
+  <si>
+    <t>Idealisatie is verplicht als Tekstdeel een locatie heeft</t>
+  </si>
+  <si>
+    <t>TPOD2120</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Iedere OW-identificatie dient uniek te zijn </t>
+  </si>
+  <si>
+    <t>TPOD2130</t>
+  </si>
+  <si>
+    <t>Iedere OW-identificatie dient slechts 1 keer voor te komen per aanlevering (c.q. je mag niet binnen dezelfde aanlevering een ID aanmaken, en vervolgens het ID wijzigen).</t>
   </si>
 </sst>
 </file>
@@ -2442,7 +2480,17 @@
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
     <cellStyle name="Standaard 2" xfId="1" xr:uid="{DD73F50D-CE68-4CBD-BD67-3376699AD112}"/>
   </cellStyles>
-  <dxfs count="123">
+  <dxfs count="124">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FFFF0000"/>
@@ -25158,247 +25206,247 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C169:F197 G167:H197 D198:D251 E198:E250 C198:C238 F198:H251 G252:H271 A28:A29 A1:E27 A152:H152 A30:F48 A59:H126 G1:V1 G2:H48 J2:J48 J59:J126 L59:L126 L2:L48 N2:N48 N59:N126 J152 J167:J271 L167:L271 L152 N152 N167:N271 P167:P271 P152 P59:P126 P2:P48 R2:R48 R59:R126 R152 T152 T59:T126 T2:T48 V2:V48 V59:V126 V152">
-    <cfRule type="containsText" dxfId="122" priority="63" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="123" priority="63" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28:E29 F1:F29">
-    <cfRule type="containsText" dxfId="121" priority="62" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="122" priority="62" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B28">
-    <cfRule type="containsText" dxfId="120" priority="61" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="121" priority="61" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B28)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B29">
-    <cfRule type="containsText" dxfId="119" priority="60" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="120" priority="60" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B29)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C252:C271">
-    <cfRule type="containsText" dxfId="118" priority="45" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="119" priority="45" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C252)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C167:F168 D252:F271">
-    <cfRule type="containsText" dxfId="117" priority="59" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="118" priority="59" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C167)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C251 E251">
-    <cfRule type="containsText" dxfId="116" priority="46" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="117" priority="46" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C251)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C239">
-    <cfRule type="containsText" dxfId="115" priority="58" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="116" priority="58" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C239)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C240">
-    <cfRule type="containsText" dxfId="114" priority="57" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="115" priority="57" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C240)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C241">
-    <cfRule type="containsText" dxfId="113" priority="56" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="114" priority="56" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C241)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C242">
-    <cfRule type="containsText" dxfId="112" priority="55" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="113" priority="55" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C242)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C243">
-    <cfRule type="containsText" dxfId="111" priority="54" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="112" priority="54" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C243)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C244">
-    <cfRule type="containsText" dxfId="110" priority="53" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="111" priority="53" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C244)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C245">
-    <cfRule type="containsText" dxfId="109" priority="52" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="110" priority="52" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C245)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C246">
-    <cfRule type="containsText" dxfId="108" priority="51" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="109" priority="51" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C246)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C247">
-    <cfRule type="containsText" dxfId="107" priority="50" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="108" priority="50" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C247)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C248">
-    <cfRule type="containsText" dxfId="106" priority="49" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="107" priority="49" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C248)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C249">
-    <cfRule type="containsText" dxfId="105" priority="48" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="106" priority="48" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C249)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C250">
-    <cfRule type="containsText" dxfId="104" priority="47" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="105" priority="47" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C250)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A49:E53 G49:H53 J49:J53 L49:L53 N49:N53 P49:P53 R49:R53 T49:T53 V49:V53">
-    <cfRule type="containsText" dxfId="103" priority="39" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="104" priority="39" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",A49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F49:F53">
-    <cfRule type="containsText" dxfId="102" priority="38" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="103" priority="38" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",F49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A54:E58 G54:H58 J54:J58 L54:L58 N54:N58 P54:P58 R54:R58 T54:T58 V54:V58">
-    <cfRule type="containsText" dxfId="101" priority="37" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="102" priority="37" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",A54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F54:F58">
-    <cfRule type="containsText" dxfId="100" priority="36" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="101" priority="36" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",F54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2:Q48 Q59:Q126 Q152">
-    <cfRule type="containsText" dxfId="99" priority="14" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="100" priority="14" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",Q2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q49:Q53">
-    <cfRule type="containsText" dxfId="98" priority="13" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="99" priority="13" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",Q49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q54:Q58">
-    <cfRule type="containsText" dxfId="97" priority="12" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="98" priority="12" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",Q54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S54:S58">
-    <cfRule type="containsText" dxfId="96" priority="9" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="97" priority="9" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",S54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U2:U48 U59:U126 U152">
-    <cfRule type="containsText" dxfId="95" priority="8" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="96" priority="8" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",U2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U49:U53">
-    <cfRule type="containsText" dxfId="94" priority="7" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="95" priority="7" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",U49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U54:U58">
-    <cfRule type="containsText" dxfId="93" priority="6" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="94" priority="6" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",U54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q167:Q271">
-    <cfRule type="containsText" dxfId="92" priority="1" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="93" priority="1" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",Q167)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I48 I59:I126 I152 I167:I271">
-    <cfRule type="containsText" dxfId="91" priority="26" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="92" priority="26" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",I2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I49:I53">
-    <cfRule type="containsText" dxfId="90" priority="25" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="91" priority="25" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",I49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I54:I58">
-    <cfRule type="containsText" dxfId="89" priority="24" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="90" priority="24" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",I54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K59:K126 K2:K48 K167:K271 K152">
-    <cfRule type="containsText" dxfId="88" priority="23" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="89" priority="23" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",K2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K49:K53">
-    <cfRule type="containsText" dxfId="87" priority="22" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="88" priority="22" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",K49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K54:K58">
-    <cfRule type="containsText" dxfId="86" priority="21" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="87" priority="21" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",K54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M48 M59:M126 M152 M167:M271">
-    <cfRule type="containsText" dxfId="85" priority="20" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="86" priority="20" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M49:M53">
-    <cfRule type="containsText" dxfId="84" priority="19" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="85" priority="19" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M54:M58">
-    <cfRule type="containsText" dxfId="83" priority="18" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="84" priority="18" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O167:O271 O152 O59:O126 O2:O48">
-    <cfRule type="containsText" dxfId="82" priority="17" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="83" priority="17" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",O2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O49:O53">
-    <cfRule type="containsText" dxfId="81" priority="16" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="82" priority="16" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",O49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O54:O58">
-    <cfRule type="containsText" dxfId="80" priority="15" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="81" priority="15" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",O54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S152 S59:S126 S2:S48">
-    <cfRule type="containsText" dxfId="79" priority="11" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="80" priority="11" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",S2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S49:S53">
-    <cfRule type="containsText" dxfId="78" priority="10" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="79" priority="10" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",S49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V167:V271 T167:T271">
-    <cfRule type="containsText" dxfId="77" priority="5" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="78" priority="5" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",T167)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U167:U271">
-    <cfRule type="containsText" dxfId="76" priority="4" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="77" priority="4" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",U167)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S167:S271">
-    <cfRule type="containsText" dxfId="75" priority="3" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="76" priority="3" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",S167)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R167:R271">
-    <cfRule type="containsText" dxfId="74" priority="2" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="75" priority="2" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",R167)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -29399,147 +29447,147 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="O2:O48">
-    <cfRule type="containsText" dxfId="73" priority="12" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="74" priority="12" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",O2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O49:O53">
-    <cfRule type="containsText" dxfId="72" priority="11" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="73" priority="11" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",O49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S2:S48">
-    <cfRule type="containsText" dxfId="71" priority="6" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="72" priority="6" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",S2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S49:S53">
-    <cfRule type="containsText" dxfId="70" priority="5" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="71" priority="5" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",S49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q49:Q53">
-    <cfRule type="containsText" dxfId="69" priority="8" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="70" priority="8" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",Q49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q54:Q58">
-    <cfRule type="containsText" dxfId="68" priority="7" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="69" priority="7" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",Q54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U54:U58">
-    <cfRule type="containsText" dxfId="67" priority="1" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="68" priority="1" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",U54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S54:S58">
-    <cfRule type="containsText" dxfId="66" priority="4" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="67" priority="4" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",S54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U2:U48">
-    <cfRule type="containsText" dxfId="65" priority="3" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="66" priority="3" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",U2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U49:U53">
-    <cfRule type="containsText" dxfId="64" priority="2" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="65" priority="2" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",U49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A28:A29 A1:E27 A30:F48 G1:V1 G2:H48 J2:J48 L2:L48 N2:N48 P2:P48 R2:R48 T2:T48 V2:V48">
-    <cfRule type="containsText" dxfId="63" priority="29" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="64" priority="29" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28:E29 F1:F29">
-    <cfRule type="containsText" dxfId="62" priority="28" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="63" priority="28" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B28">
-    <cfRule type="containsText" dxfId="61" priority="27" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="62" priority="27" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B28)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B29">
-    <cfRule type="containsText" dxfId="60" priority="26" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="61" priority="26" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B29)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A49:E53 G49:H53 J49:J53 L49:L53 N49:N53 P49:P53 R49:R53 T49:T53 V49:V53">
-    <cfRule type="containsText" dxfId="59" priority="25" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="60" priority="25" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",A49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F49:F53">
-    <cfRule type="containsText" dxfId="58" priority="24" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="59" priority="24" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",F49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A54:E58 G54:H58 J54:J58 L54:L58 N54:N58 P54:P58 R54:R58 T54:T58 V54:V58">
-    <cfRule type="containsText" dxfId="57" priority="23" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="58" priority="23" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",A54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F54:F58">
-    <cfRule type="containsText" dxfId="56" priority="22" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="57" priority="22" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",F54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2:Q48">
-    <cfRule type="containsText" dxfId="55" priority="9" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="56" priority="9" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",Q2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I48">
-    <cfRule type="containsText" dxfId="54" priority="21" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="55" priority="21" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",I2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I49:I53">
-    <cfRule type="containsText" dxfId="53" priority="20" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="54" priority="20" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",I49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I54:I58">
-    <cfRule type="containsText" dxfId="52" priority="19" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="53" priority="19" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",I54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K48">
-    <cfRule type="containsText" dxfId="51" priority="18" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="52" priority="18" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",K2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K49:K53">
-    <cfRule type="containsText" dxfId="50" priority="17" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="51" priority="17" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",K49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K54:K58">
-    <cfRule type="containsText" dxfId="49" priority="16" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="50" priority="16" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",K54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M48">
-    <cfRule type="containsText" dxfId="48" priority="15" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="49" priority="15" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M49:M53">
-    <cfRule type="containsText" dxfId="47" priority="14" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="48" priority="14" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M54:M58">
-    <cfRule type="containsText" dxfId="46" priority="13" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="47" priority="13" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O54:O58">
-    <cfRule type="containsText" dxfId="45" priority="10" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="46" priority="10" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",O54)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -29568,9 +29616,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{511BE904-3D15-4F6E-B5B9-2AD212EB1E09}">
   <dimension ref="A1:W217"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B117" sqref="B117"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I120" sqref="I120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -37475,23 +37523,413 @@
         <v>134</v>
       </c>
     </row>
-    <row r="118" spans="2:23" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="B118" s="45"/>
-    </row>
-    <row r="119" spans="2:23" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="B119" s="45"/>
-    </row>
-    <row r="120" spans="2:23" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="B120" s="45"/>
-    </row>
-    <row r="121" spans="2:23" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="B121" s="45"/>
-    </row>
-    <row r="122" spans="2:23" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="B122" s="45"/>
-    </row>
-    <row r="123" spans="2:23" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="B123" s="45"/>
+    <row r="118" spans="2:23" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="B118" s="1" t="s">
+        <v>680</v>
+      </c>
+      <c r="C118" s="55" t="s">
+        <v>681</v>
+      </c>
+      <c r="D118" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="E118" s="3" t="s">
+        <v>682</v>
+      </c>
+      <c r="F118" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="G118" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="H118" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="I118" s="3" t="s">
+        <v>643</v>
+      </c>
+      <c r="J118" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="K118" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="L118" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="M118" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="N118" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="O118" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="P118" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q118" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="R118" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="S118" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="T118" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="U118" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="V118" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="W118" s="19" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="119" spans="2:23" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="B119" s="1" t="s">
+        <v>683</v>
+      </c>
+      <c r="C119" s="55" t="s">
+        <v>684</v>
+      </c>
+      <c r="D119" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="E119" s="3" t="s">
+        <v>682</v>
+      </c>
+      <c r="F119" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="G119" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="H119" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="I119" s="3" t="s">
+        <v>643</v>
+      </c>
+      <c r="J119" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="K119" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="L119" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="M119" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="N119" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="O119" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="P119" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q119" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="R119" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="S119" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="T119" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="U119" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="V119" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="W119" s="19" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="120" spans="2:23" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="B120" s="1" t="s">
+        <v>685</v>
+      </c>
+      <c r="C120" s="55" t="s">
+        <v>686</v>
+      </c>
+      <c r="D120" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="E120" s="3" t="s">
+        <v>682</v>
+      </c>
+      <c r="F120" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="G120" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="H120" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="I120" s="3" t="s">
+        <v>643</v>
+      </c>
+      <c r="J120" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="K120" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="L120" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="M120" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="N120" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="O120" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="P120" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q120" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="R120" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="S120" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="T120" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="U120" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="V120" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="W120" s="19" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="121" spans="2:23" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="B121" s="1" t="s">
+        <v>687</v>
+      </c>
+      <c r="C121" s="55" t="s">
+        <v>688</v>
+      </c>
+      <c r="D121" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="E121" s="3" t="s">
+        <v>682</v>
+      </c>
+      <c r="F121" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="G121" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="H121" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="I121" s="3" t="s">
+        <v>643</v>
+      </c>
+      <c r="J121" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="K121" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="L121" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="M121" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="N121" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="O121" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="P121" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q121" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="R121" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="S121" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="T121" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="U121" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="V121" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="W121" s="19" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="122" spans="2:23" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="B122" s="1" t="s">
+        <v>689</v>
+      </c>
+      <c r="C122" s="55" t="s">
+        <v>690</v>
+      </c>
+      <c r="D122" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="E122" s="3" t="s">
+        <v>682</v>
+      </c>
+      <c r="F122" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="G122" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="H122" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="I122" s="3" t="s">
+        <v>643</v>
+      </c>
+      <c r="J122" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="K122" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="L122" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="M122" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="N122" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="O122" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="P122" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q122" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="R122" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="S122" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="T122" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="U122" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="V122" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="W122" s="19" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="123" spans="2:23" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="B123" s="1" t="s">
+        <v>691</v>
+      </c>
+      <c r="C123" s="55" t="s">
+        <v>692</v>
+      </c>
+      <c r="D123" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="E123" s="3" t="s">
+        <v>682</v>
+      </c>
+      <c r="F123" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="G123" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="H123" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="I123" s="3" t="s">
+        <v>643</v>
+      </c>
+      <c r="J123" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="K123" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="L123" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="M123" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="N123" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="O123" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="P123" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q123" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="R123" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="S123" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="T123" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="U123" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="V123" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="W123" s="19" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="124" spans="2:23" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B124" s="45"/>
@@ -37777,63 +38215,68 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B96:I96 B2:I69">
-    <cfRule type="containsText" dxfId="44" priority="24" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="45" priority="25" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T95 T2:T69">
-    <cfRule type="containsText" dxfId="43" priority="2" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="44" priority="3" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",T2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V2:V69 V95">
-    <cfRule type="containsText" dxfId="42" priority="1" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="43" priority="2" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",V2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:F1 H1:W1">
-    <cfRule type="containsText" dxfId="41" priority="20" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="42" priority="21" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1">
-    <cfRule type="containsText" dxfId="40" priority="19" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="41" priority="20" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B202 B118:B176">
-    <cfRule type="containsText" dxfId="39" priority="18" operator="containsText" text="&lt;?&gt;">
-      <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B118)))</formula>
+  <conditionalFormatting sqref="B202 B124:B176">
+    <cfRule type="containsText" dxfId="40" priority="19" operator="containsText" text="&lt;?&gt;">
+      <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B124)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K69 M2:M69 O2:O69 K95 M95 O95 Q95 Q2:Q69 S2:S69 S95 U95 U2:U69 W2:W69 W95">
-    <cfRule type="containsText" dxfId="38" priority="8" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="39" priority="9" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",K2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R2:R69 R95">
-    <cfRule type="containsText" dxfId="37" priority="3" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="38" priority="4" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",R2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J69 J95">
-    <cfRule type="containsText" dxfId="36" priority="7" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="37" priority="8" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",J2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:L69 L95">
-    <cfRule type="containsText" dxfId="35" priority="6" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="36" priority="7" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",L2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2:N69 N95">
-    <cfRule type="containsText" dxfId="34" priority="5" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="35" priority="6" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",N2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P95 P2:P69">
-    <cfRule type="containsText" dxfId="33" priority="4" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="34" priority="5" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",P2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B118:B123">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="&lt;?&gt;">
+      <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B118)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -45088,137 +45531,137 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:E1 G1:H1">
-    <cfRule type="containsText" dxfId="32" priority="27" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="33" priority="27" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1">
-    <cfRule type="containsText" dxfId="31" priority="26" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="32" priority="26" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",F1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:F32 D33:D86 E33:E85 C33:C73 G2:H32 F33:H86 G87:H106 V2:V106 T2:T106 R2:R106">
-    <cfRule type="containsText" dxfId="30" priority="25" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="31" priority="25" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C87:C106">
-    <cfRule type="containsText" dxfId="29" priority="10" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="30" priority="10" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C87)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:F3 D87:F106">
-    <cfRule type="containsText" dxfId="28" priority="24" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="29" priority="24" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C86 E86">
-    <cfRule type="containsText" dxfId="27" priority="11" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="28" priority="11" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C86)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C74">
-    <cfRule type="containsText" dxfId="26" priority="23" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="27" priority="23" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C74)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C75">
-    <cfRule type="containsText" dxfId="25" priority="22" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="26" priority="22" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C75)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C76">
-    <cfRule type="containsText" dxfId="24" priority="21" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="25" priority="21" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C76)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C77">
-    <cfRule type="containsText" dxfId="23" priority="20" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="24" priority="20" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C77)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C78">
-    <cfRule type="containsText" dxfId="22" priority="19" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="23" priority="19" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C78)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C79">
-    <cfRule type="containsText" dxfId="21" priority="18" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="22" priority="18" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C79)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C80">
-    <cfRule type="containsText" dxfId="20" priority="17" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="21" priority="17" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C80)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C81">
-    <cfRule type="containsText" dxfId="19" priority="16" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="20" priority="16" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C81)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C82">
-    <cfRule type="containsText" dxfId="18" priority="15" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="19" priority="15" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C82)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C83">
-    <cfRule type="containsText" dxfId="17" priority="14" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="18" priority="14" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C83)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C84">
-    <cfRule type="containsText" dxfId="16" priority="13" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="17" priority="13" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C84)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C85">
-    <cfRule type="containsText" dxfId="15" priority="12" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="16" priority="12" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C85)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:V1">
-    <cfRule type="containsText" dxfId="14" priority="9" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="15" priority="9" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",I1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U2:U106">
-    <cfRule type="containsText" dxfId="13" priority="8" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="14" priority="8" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",U2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S2:S106">
-    <cfRule type="containsText" dxfId="12" priority="7" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="13" priority="7" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",S2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2:Q106">
-    <cfRule type="containsText" dxfId="11" priority="6" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="12" priority="6" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",Q2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J106 L2:L106 N2:N106 P2:P106">
-    <cfRule type="containsText" dxfId="10" priority="5" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="11" priority="5" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",J2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I106">
-    <cfRule type="containsText" dxfId="9" priority="4" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="10" priority="4" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",I2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K106">
-    <cfRule type="containsText" dxfId="8" priority="3" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="9" priority="3" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",K2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M106">
-    <cfRule type="containsText" dxfId="7" priority="2" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="8" priority="2" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O2:O106">
-    <cfRule type="containsText" dxfId="6" priority="1" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="7" priority="1" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",O2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -46075,17 +46518,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:E1 G1:H1">
-    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="6" priority="4" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1">
-    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",F1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:V1">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",I1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -48224,17 +48667,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:E1 G1:H1">
-    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1">
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",F1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:V1">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",I1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
vergeleken met het bestand dat erik publiceert (verder geen wijzigingen w.m.b. ,maar excel vond van wel).
</commit_message>
<xml_diff>
--- a/1.0-Validatie-_en_conformiteitsregels_TPOD/documentatie/Validatie-en-Conformiteitsregels Totaal v0.10 - incl onderscheidOntwerpDefinitief.xlsx
+++ b/1.0-Validatie-_en_conformiteitsregels_TPOD/documentatie/Validatie-en-Conformiteitsregels Totaal v0.10 - incl onderscheidOntwerpDefinitief.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RicharddeGraaf\Desktop\Geonovum\4 - Voorbeeldbestanden\GITHub\xml_schematron\1.0-Validatie-_en_conformiteitsregels_TPOD\documentatie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23E170EE-850C-4895-99F7-B6D9A0F53CB9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4605BD87-8B1E-4BF1-BFA5-3DFC50072D22}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{CAF58E0D-33FE-46EB-ADA3-90D1B902B379}"/>
   </bookViews>
@@ -19,6 +19,9 @@
   <externalReferences>
     <externalReference r:id="rId3"/>
   </externalReferences>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">TPOD!$A$1:$Y$122</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -2757,27 +2760,7 @@
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
     <cellStyle name="Standaard 2" xfId="1" xr:uid="{DD73F50D-CE68-4CBD-BD67-3376699AD112}"/>
   </cellStyles>
-  <dxfs count="63">
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="61">
     <dxf>
       <font>
         <color rgb="FFFF0000"/>
@@ -3714,7 +3697,7 @@
   <dimension ref="A1:V312"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A167" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B70" sqref="B70"/>
     </sheetView>
   </sheetViews>
@@ -24873,247 +24856,247 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C169:F197 G167:H197 D198:D251 E198:E250 C198:C238 F198:H251 G252:H271 A28:A29 A1:E27 A152:H152 A30:F48 A59:H126 G1:V1 G2:H48 J2:J48 J59:J126 L59:L126 L2:L48 N2:N48 N59:N126 J152 J167:J271 L167:L271 L152 N152 N167:N271 P167:P271 P152 P59:P126 P2:P48 R2:R48 R59:R126 R152 T152 T59:T126 T2:T48 V2:V48 V59:V126 V152">
-    <cfRule type="containsText" dxfId="62" priority="63" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="60" priority="63" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28:E29 F1:F29">
-    <cfRule type="containsText" dxfId="61" priority="62" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="59" priority="62" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B28">
-    <cfRule type="containsText" dxfId="60" priority="61" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="58" priority="61" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B28)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B29">
-    <cfRule type="containsText" dxfId="59" priority="60" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="57" priority="60" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B29)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C252:C271">
-    <cfRule type="containsText" dxfId="58" priority="45" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="56" priority="45" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C252)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C167:F168 D252:F271">
-    <cfRule type="containsText" dxfId="57" priority="59" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="55" priority="59" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C167)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C251 E251">
-    <cfRule type="containsText" dxfId="56" priority="46" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="54" priority="46" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C251)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C239">
-    <cfRule type="containsText" dxfId="55" priority="58" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="53" priority="58" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C239)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C240">
-    <cfRule type="containsText" dxfId="54" priority="57" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="52" priority="57" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C240)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C241">
-    <cfRule type="containsText" dxfId="53" priority="56" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="51" priority="56" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C241)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C242">
-    <cfRule type="containsText" dxfId="52" priority="55" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="50" priority="55" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C242)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C243">
-    <cfRule type="containsText" dxfId="51" priority="54" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="49" priority="54" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C243)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C244">
-    <cfRule type="containsText" dxfId="50" priority="53" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="48" priority="53" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C244)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C245">
-    <cfRule type="containsText" dxfId="49" priority="52" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="47" priority="52" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C245)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C246">
-    <cfRule type="containsText" dxfId="48" priority="51" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="46" priority="51" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C246)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C247">
-    <cfRule type="containsText" dxfId="47" priority="50" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="45" priority="50" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C247)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C248">
-    <cfRule type="containsText" dxfId="46" priority="49" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="44" priority="49" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C248)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C249">
-    <cfRule type="containsText" dxfId="45" priority="48" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="43" priority="48" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C249)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C250">
-    <cfRule type="containsText" dxfId="44" priority="47" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="42" priority="47" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C250)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A49:E53 G49:H53 J49:J53 L49:L53 N49:N53 P49:P53 R49:R53 T49:T53 V49:V53">
-    <cfRule type="containsText" dxfId="43" priority="39" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="41" priority="39" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",A49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F49:F53">
-    <cfRule type="containsText" dxfId="42" priority="38" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="40" priority="38" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",F49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A54:E58 G54:H58 J54:J58 L54:L58 N54:N58 P54:P58 R54:R58 T54:T58 V54:V58">
-    <cfRule type="containsText" dxfId="41" priority="37" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="39" priority="37" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",A54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F54:F58">
-    <cfRule type="containsText" dxfId="40" priority="36" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="38" priority="36" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",F54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2:Q48 Q59:Q126 Q152">
-    <cfRule type="containsText" dxfId="39" priority="14" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="37" priority="14" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",Q2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q49:Q53">
-    <cfRule type="containsText" dxfId="38" priority="13" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="36" priority="13" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",Q49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q54:Q58">
-    <cfRule type="containsText" dxfId="37" priority="12" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="35" priority="12" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",Q54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S54:S58">
-    <cfRule type="containsText" dxfId="36" priority="9" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="34" priority="9" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",S54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U2:U48 U59:U126 U152">
-    <cfRule type="containsText" dxfId="35" priority="8" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="33" priority="8" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",U2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U49:U53">
-    <cfRule type="containsText" dxfId="34" priority="7" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="32" priority="7" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",U49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U54:U58">
-    <cfRule type="containsText" dxfId="33" priority="6" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="31" priority="6" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",U54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q167:Q271">
-    <cfRule type="containsText" dxfId="32" priority="1" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="30" priority="1" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",Q167)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I48 I59:I126 I152 I167:I271">
-    <cfRule type="containsText" dxfId="31" priority="26" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="29" priority="26" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",I2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I49:I53">
-    <cfRule type="containsText" dxfId="30" priority="25" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="28" priority="25" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",I49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I54:I58">
-    <cfRule type="containsText" dxfId="29" priority="24" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="27" priority="24" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",I54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K59:K126 K2:K48 K167:K271 K152">
-    <cfRule type="containsText" dxfId="28" priority="23" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="26" priority="23" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",K2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K49:K53">
-    <cfRule type="containsText" dxfId="27" priority="22" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="25" priority="22" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",K49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K54:K58">
-    <cfRule type="containsText" dxfId="26" priority="21" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="24" priority="21" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",K54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M48 M59:M126 M152 M167:M271">
-    <cfRule type="containsText" dxfId="25" priority="20" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="23" priority="20" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M49:M53">
-    <cfRule type="containsText" dxfId="24" priority="19" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="22" priority="19" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M54:M58">
-    <cfRule type="containsText" dxfId="23" priority="18" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="21" priority="18" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O167:O271 O152 O59:O126 O2:O48">
-    <cfRule type="containsText" dxfId="22" priority="17" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="20" priority="17" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",O2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O49:O53">
-    <cfRule type="containsText" dxfId="21" priority="16" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="19" priority="16" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",O49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O54:O58">
-    <cfRule type="containsText" dxfId="20" priority="15" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="18" priority="15" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",O54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S152 S59:S126 S2:S48">
-    <cfRule type="containsText" dxfId="19" priority="11" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="17" priority="11" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",S2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S49:S53">
-    <cfRule type="containsText" dxfId="18" priority="10" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="16" priority="10" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",S49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V167:V271 T167:T271">
-    <cfRule type="containsText" dxfId="17" priority="5" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="15" priority="5" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",T167)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U167:U271">
-    <cfRule type="containsText" dxfId="16" priority="4" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="14" priority="4" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",U167)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S167:S271">
-    <cfRule type="containsText" dxfId="15" priority="3" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="13" priority="3" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",S167)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R167:R271">
-    <cfRule type="containsText" dxfId="14" priority="2" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="12" priority="2" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",R167)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -25153,8 +25136,8 @@
   <dimension ref="A1:Y122"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A116" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C120" sqref="C120"/>
+      <pane ySplit="1" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C108" sqref="C108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -34563,53 +34546,54 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:Y122" xr:uid="{9EE4866E-E834-4DB8-9ED6-70561D41353B}"/>
   <conditionalFormatting sqref="M2:M69 O2:O69 Q2:Q69 M95 O95 Q95 S95 S2:S69 U2:U69 U95 W95 W2:W69 Y2:Y69 Y95 A2:A122">
-    <cfRule type="containsText" dxfId="13" priority="15" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="11" priority="15" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",A2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2:N69 N95">
-    <cfRule type="containsText" dxfId="12" priority="13" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="10" priority="13" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",N2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:L69 L95">
-    <cfRule type="containsText" dxfId="11" priority="14" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="9" priority="14" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",L2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D96:K96 D2:K69">
-    <cfRule type="containsText" dxfId="10" priority="16" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="8" priority="16" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Y1">
-    <cfRule type="containsText" dxfId="9" priority="25" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="7" priority="25" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R95 R2:R69">
-    <cfRule type="containsText" dxfId="8" priority="11" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="6" priority="11" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",R2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T2:T69 T95">
-    <cfRule type="containsText" dxfId="7" priority="10" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="5" priority="10" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",T2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V95 V2:V69">
-    <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="4" priority="9" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",V2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X2:X69 X95">
-    <cfRule type="containsText" dxfId="5" priority="8" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="3" priority="8" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",X2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P2:P69 P95">
-    <cfRule type="containsText" dxfId="4" priority="12" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="2" priority="12" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",P2)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>